<commit_message>
Results from July 07, 2020 09:10:33 AM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-07.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-07.xlsx
@@ -979,25 +979,25 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44017</v>
+        <v>44019</v>
       </c>
       <c r="C11" t="n">
-        <v>65748</v>
+        <v>66740</v>
       </c>
       <c r="D11" t="n">
-        <v>1853</v>
+        <v>1881</v>
       </c>
       <c r="E11" t="n">
-        <v>9541</v>
+        <v>9747</v>
       </c>
       <c r="F11" t="n">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="G11" t="n">
-        <v>14.51</v>
+        <v>14.6</v>
       </c>
       <c r="H11" t="n">
-        <v>22.29</v>
+        <v>22.22</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -1261,25 +1261,25 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C17" t="n">
-        <v>69904</v>
+        <v>70396</v>
       </c>
       <c r="D17" t="n">
-        <v>3121</v>
+        <v>3140</v>
       </c>
       <c r="E17" t="n">
-        <v>20043</v>
+        <v>20157</v>
       </c>
       <c r="F17" t="n">
-        <v>1263</v>
+        <v>1266</v>
       </c>
       <c r="G17" t="n">
-        <v>28.67</v>
+        <v>28.63</v>
       </c>
       <c r="H17" t="n">
-        <v>40.47</v>
+        <v>40.32</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1288,10 +1288,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>57246</v>
+        <v>57574</v>
       </c>
       <c r="L17" t="n">
-        <v>69882</v>
+        <v>70366</v>
       </c>
       <c r="M17" t="n">
         <v>1788090</v>
@@ -1998,25 +1998,25 @@
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44017</v>
+        <v>44019</v>
       </c>
       <c r="C32" t="n">
-        <v>10482</v>
+        <v>10569</v>
       </c>
       <c r="D32" t="n">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="E32" t="n">
-        <v>5213</v>
+        <v>5241</v>
       </c>
       <c r="F32" t="n">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="G32" t="n">
-        <v>49.73</v>
+        <v>49.59</v>
       </c>
       <c r="H32" t="n">
-        <v>73.7</v>
+        <v>74.51000000000001</v>
       </c>
       <c r="I32" t="b">
         <v>1</v>
@@ -2092,20 +2092,20 @@
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C34" t="n">
-        <v>3423</v>
+        <v>3440</v>
       </c>
       <c r="D34" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E34" t="n">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
-        <v>26.52</v>
+        <v>26.42</v>
       </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="b">
@@ -2115,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>3028</v>
+        <v>3036</v>
       </c>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="n">

</xml_diff>

<commit_message>
Results from July 07, 2020 09:15:09 AM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-07.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-07.xlsx
@@ -2477,18 +2477,32 @@
           <t>Iowa</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+      <c r="B42" s="2" t="n">
+        <v>44019</v>
+      </c>
+      <c r="C42" t="n">
+        <v>31906</v>
+      </c>
+      <c r="D42" t="n">
+        <v>725</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2868</v>
+      </c>
+      <c r="F42" t="n">
+        <v>36</v>
+      </c>
+      <c r="G42" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="H42" t="n">
+        <v>4.97</v>
+      </c>
       <c r="I42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
@@ -2500,7 +2514,7 @@
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>An error occurred. ... ValueError('Unable to parse "Reported Deaths In Adair : No Data" as int')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 07, 2020 07:58:16 PM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-07.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-07.xlsx
@@ -522,19 +522,19 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C2" t="n">
-        <v>23242</v>
+        <v>23607</v>
       </c>
       <c r="D2" t="n">
-        <v>680</v>
+        <v>689</v>
       </c>
       <c r="E2" t="n">
-        <v>2721</v>
+        <v>2747</v>
       </c>
       <c r="F2" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G2" t="n">
         <v>0.12</v>
@@ -569,13 +569,13 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C3" t="n">
-        <v>15102</v>
+        <v>15880</v>
       </c>
       <c r="D3" t="n">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E3" t="n">
         <v>464</v>
@@ -620,29 +620,29 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>214061</t>
+          <t>214371</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18596</t>
+          <t>18611</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>33265</v>
+        <v>33277</v>
       </c>
       <c r="F4" t="n">
-        <v>5199</v>
+        <v>5206</v>
       </c>
       <c r="G4" t="n">
         <v>30.16</v>
       </c>
       <c r="H4" t="n">
-        <v>30.5</v>
+        <v>30.51</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -651,10 +651,10 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>110283</v>
+        <v>110332</v>
       </c>
       <c r="L4" t="n">
-        <v>17048</v>
+        <v>17065</v>
       </c>
       <c r="M4" t="n">
         <v>2049418</v>
@@ -726,25 +726,25 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C6" t="n">
-        <v>52155</v>
+        <v>53514</v>
       </c>
       <c r="D6" t="n">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="E6" t="n">
-        <v>10640</v>
+        <v>10872</v>
       </c>
       <c r="F6" t="n">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="G6" t="n">
-        <v>20.4</v>
+        <v>20.32</v>
       </c>
       <c r="H6" t="n">
-        <v>35.38</v>
+        <v>35.19</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -773,21 +773,21 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>25469</t>
+          <t>26033</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>189</t>
+          <t>194</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>657</t>
+          <t>666</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -826,25 +826,25 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C8" t="n">
-        <v>17152</v>
+        <v>17519</v>
       </c>
       <c r="D8" t="n">
-        <v>593</v>
+        <v>602</v>
       </c>
       <c r="E8" t="n">
-        <v>1650</v>
+        <v>1675</v>
       </c>
       <c r="F8" t="n">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="G8" t="n">
-        <v>14.14</v>
+        <v>13.64</v>
       </c>
       <c r="H8" t="n">
-        <v>4.14</v>
+        <v>15.43</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
@@ -853,10 +853,10 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>11675</v>
+        <v>12280</v>
       </c>
       <c r="L8" t="n">
-        <v>554</v>
+        <v>564</v>
       </c>
       <c r="M8" t="n">
         <v>354112</v>
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C9" t="n">
         <v>24253</v>
@@ -928,25 +928,25 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C10" t="n">
-        <v>17000</v>
+        <v>17578</v>
       </c>
       <c r="D10" t="n">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="E10" t="n">
-        <v>615</v>
+        <v>635</v>
       </c>
       <c r="F10" t="n">
         <v>13</v>
       </c>
       <c r="G10" t="n">
-        <v>4.55</v>
+        <v>4.57</v>
       </c>
       <c r="H10" t="n">
-        <v>3.4</v>
+        <v>3.32</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -955,10 +955,10 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>13514</v>
+        <v>13892</v>
       </c>
       <c r="L10" t="n">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="M10" t="n">
         <v>166412</v>
@@ -1026,20 +1026,20 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C12" t="n">
-        <v>13507</v>
+        <v>13727</v>
       </c>
       <c r="D12" t="n">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="E12" t="n">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>1.92</v>
+        <v>1.9</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="b">
@@ -1069,20 +1069,20 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C13" t="n">
-        <v>48992</v>
+        <v>51058</v>
       </c>
       <c r="D13" t="n">
-        <v>1051</v>
+        <v>1057</v>
       </c>
       <c r="E13" t="n">
-        <v>5897</v>
+        <v>6050</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>21.03</v>
+        <v>20.55</v>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="b">
@@ -1092,7 +1092,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>28046</v>
+        <v>29436</v>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
@@ -1114,20 +1114,20 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C14" t="n">
-        <v>14407</v>
+        <v>14768</v>
       </c>
       <c r="D14" t="n">
         <v>61</v>
       </c>
       <c r="E14" t="n">
-        <v>1842</v>
+        <v>1902</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>24.03</v>
+        <v>24.07</v>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="b">
@@ -1137,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>7664</v>
+        <v>7901</v>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
@@ -1159,25 +1159,25 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C15" t="n">
-        <v>44375</v>
+        <v>45263</v>
       </c>
       <c r="D15" t="n">
-        <v>984</v>
+        <v>1007</v>
       </c>
       <c r="E15" t="n">
-        <v>15481</v>
+        <v>15769</v>
       </c>
       <c r="F15" t="n">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="G15" t="n">
-        <v>46.61</v>
+        <v>46.33</v>
       </c>
       <c r="H15" t="n">
-        <v>46.48</v>
+        <v>46.35</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
@@ -1186,10 +1186,10 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>33213</v>
+        <v>34039</v>
       </c>
       <c r="L15" t="n">
-        <v>951</v>
+        <v>973</v>
       </c>
       <c r="M15" t="n">
         <v>1293186</v>
@@ -1210,25 +1210,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C16" t="n">
-        <v>116570</v>
+        <v>120539</v>
       </c>
       <c r="D16" t="n">
-        <v>3534</v>
+        <v>3579</v>
       </c>
       <c r="E16" t="n">
-        <v>3170</v>
+        <v>3232</v>
       </c>
       <c r="F16" t="n">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G16" t="n">
         <v>4.7</v>
       </c>
       <c r="H16" t="n">
-        <v>11.21</v>
+        <v>11.09</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1237,10 +1237,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>67498</v>
+        <v>68774</v>
       </c>
       <c r="L16" t="n">
-        <v>3283</v>
+        <v>3327</v>
       </c>
       <c r="M16" t="n">
         <v>823987</v>
@@ -1312,25 +1312,25 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C18" t="n">
-        <v>31257</v>
+        <v>32214</v>
       </c>
       <c r="D18" t="n">
-        <v>1114</v>
+        <v>1158</v>
       </c>
       <c r="E18" t="n">
-        <v>15110</v>
+        <v>15391</v>
       </c>
       <c r="F18" t="n">
-        <v>558</v>
+        <v>579</v>
       </c>
       <c r="G18" t="n">
-        <v>48.34</v>
+        <v>47.78</v>
       </c>
       <c r="H18" t="n">
-        <v>50.09</v>
+        <v>50</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -1359,22 +1359,22 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C19" t="n">
-        <v>87705</v>
+        <v>88691</v>
       </c>
       <c r="D19" t="n">
-        <v>6754</v>
+        <v>6787</v>
       </c>
       <c r="E19" t="n">
-        <v>11603</v>
+        <v>11754</v>
       </c>
       <c r="F19" t="n">
         <v>1426</v>
       </c>
       <c r="G19" t="n">
-        <v>30.05</v>
+        <v>30.08</v>
       </c>
       <c r="H19" t="n">
         <v>21.68</v>
@@ -1386,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>38615</v>
+        <v>39071</v>
       </c>
       <c r="L19" t="n">
         <v>6579</v>
@@ -1410,25 +1410,25 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C20" t="n">
-        <v>203376</v>
+        <v>210594</v>
       </c>
       <c r="D20" t="n">
-        <v>3778</v>
+        <v>3841</v>
       </c>
       <c r="E20" t="n">
-        <v>26511</v>
+        <v>27447</v>
       </c>
       <c r="F20" t="n">
-        <v>737</v>
+        <v>753</v>
       </c>
       <c r="G20" t="n">
-        <v>13.04</v>
+        <v>13.03</v>
       </c>
       <c r="H20" t="n">
-        <v>19.51</v>
+        <v>19.6</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -1457,10 +1457,10 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C21" t="n">
-        <v>1249</v>
+        <v>1327</v>
       </c>
       <c r="D21" t="n">
         <v>23</v>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>0.48</v>
+        <v>0.45</v>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="b">
@@ -1500,22 +1500,22 @@
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C22" t="n">
-        <v>1251</v>
+        <v>1254</v>
       </c>
       <c r="D22" t="n">
         <v>56</v>
       </c>
       <c r="E22" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>10.44</v>
+        <v>10.49</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1527,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>1217</v>
+        <v>1220</v>
       </c>
       <c r="L22" t="n">
         <v>56</v>
@@ -1551,16 +1551,16 @@
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C23" t="n">
-        <v>34257</v>
+        <v>34664</v>
       </c>
       <c r="D23" t="n">
-        <v>1691</v>
+        <v>1696</v>
       </c>
       <c r="E23" t="n">
-        <v>1809</v>
+        <v>1827</v>
       </c>
       <c r="F23" t="n">
         <v>110</v>
@@ -1569,7 +1569,7 @@
         <v>6.42</v>
       </c>
       <c r="H23" t="n">
-        <v>6.76</v>
+        <v>6.73</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
@@ -1578,10 +1578,10 @@
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>28159</v>
+        <v>28456</v>
       </c>
       <c r="L23" t="n">
-        <v>1628</v>
+        <v>1634</v>
       </c>
       <c r="M23" t="n">
         <v>227938</v>
@@ -1602,22 +1602,22 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C24" t="n">
-        <v>20046</v>
+        <v>20201</v>
       </c>
       <c r="D24" t="n">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E24" t="n">
-        <v>1184</v>
+        <v>1200</v>
       </c>
       <c r="F24" t="n">
         <v>21</v>
       </c>
       <c r="G24" t="n">
-        <v>7.65</v>
+        <v>7.67</v>
       </c>
       <c r="H24" t="n">
         <v>7.72</v>
@@ -1629,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>15470</v>
+        <v>15643</v>
       </c>
       <c r="L24" t="n">
         <v>272</v>
@@ -1653,25 +1653,25 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C25" t="n">
-        <v>66089</v>
+        <v>66540</v>
       </c>
       <c r="D25" t="n">
-        <v>5897</v>
+        <v>5926</v>
       </c>
       <c r="E25" t="n">
-        <v>19987</v>
+        <v>20100</v>
       </c>
       <c r="F25" t="n">
-        <v>2358</v>
+        <v>2364</v>
       </c>
       <c r="G25" t="n">
-        <v>30.24</v>
+        <v>30.21</v>
       </c>
       <c r="H25" t="n">
-        <v>39.99</v>
+        <v>39.89</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -1700,22 +1700,22 @@
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C26" t="n">
-        <v>271684</v>
+        <v>277774</v>
       </c>
       <c r="D26" t="n">
-        <v>6300</v>
+        <v>6361</v>
       </c>
       <c r="E26" t="n">
-        <v>7693</v>
+        <v>7869</v>
       </c>
       <c r="F26" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="G26" t="n">
-        <v>4.3</v>
+        <v>4.4</v>
       </c>
       <c r="H26" t="n">
         <v>9.199999999999999</v>
@@ -1727,10 +1727,10 @@
         <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>177012</v>
+        <v>180178</v>
       </c>
       <c r="L26" t="n">
-        <v>6227</v>
+        <v>6282</v>
       </c>
       <c r="M26" t="n">
         <v>2267875</v>
@@ -1751,25 +1751,25 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C27" t="n">
-        <v>48331</v>
+        <v>48626</v>
       </c>
       <c r="D27" t="n">
-        <v>2505</v>
+        <v>2524</v>
       </c>
       <c r="E27" t="n">
-        <v>5798</v>
+        <v>5883</v>
       </c>
       <c r="F27" t="n">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="G27" t="n">
-        <v>12</v>
+        <v>12.1</v>
       </c>
       <c r="H27" t="n">
-        <v>14.49</v>
+        <v>14.54</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -1798,22 +1798,22 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C28" t="n">
-        <v>1166</v>
+        <v>1184</v>
       </c>
       <c r="D28" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E28" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>1.23</v>
+        <v>1.4</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -1825,10 +1825,10 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>2026</v>
+        <v>2069</v>
       </c>
       <c r="L28" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M28" t="n">
         <v>24129</v>
@@ -1849,25 +1849,25 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C29" t="n">
-        <v>32061</v>
+        <v>32556</v>
       </c>
       <c r="D29" t="n">
-        <v>796</v>
+        <v>805</v>
       </c>
       <c r="E29" t="n">
-        <v>5487</v>
+        <v>5560</v>
       </c>
       <c r="F29" t="n">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G29" t="n">
-        <v>19.04</v>
+        <v>18.97</v>
       </c>
       <c r="H29" t="n">
-        <v>23.95</v>
+        <v>24.21</v>
       </c>
       <c r="I29" t="b">
         <v>0</v>
@@ -1876,10 +1876,10 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>28819</v>
+        <v>29315</v>
       </c>
       <c r="L29" t="n">
-        <v>785</v>
+        <v>793</v>
       </c>
       <c r="M29" t="n">
         <v>368744</v>
@@ -1900,25 +1900,25 @@
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C30" t="n">
-        <v>97064</v>
+        <v>100470</v>
       </c>
       <c r="D30" t="n">
-        <v>2878</v>
+        <v>2899</v>
       </c>
       <c r="E30" t="n">
-        <v>26887</v>
+        <v>27660</v>
       </c>
       <c r="F30" t="n">
-        <v>1357</v>
+        <v>1361</v>
       </c>
       <c r="G30" t="n">
-        <v>27.7</v>
+        <v>27.53</v>
       </c>
       <c r="H30" t="n">
-        <v>47.15</v>
+        <v>46.95</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
@@ -1947,25 +1947,25 @@
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C31" t="n">
-        <v>36985</v>
+        <v>37420</v>
       </c>
       <c r="D31" t="n">
-        <v>1370</v>
+        <v>1384</v>
       </c>
       <c r="E31" t="n">
-        <v>1455</v>
+        <v>1464</v>
       </c>
       <c r="F31" t="n">
         <v>45</v>
       </c>
       <c r="G31" t="n">
-        <v>5.49</v>
+        <v>5.48</v>
       </c>
       <c r="H31" t="n">
-        <v>3.46</v>
+        <v>3.43</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
@@ -1974,10 +1974,10 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>26515</v>
+        <v>26717</v>
       </c>
       <c r="L31" t="n">
-        <v>1301</v>
+        <v>1312</v>
       </c>
       <c r="M31" t="n">
         <v>269854</v>
@@ -2045,25 +2045,25 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C33" t="n">
-        <v>12293</v>
+        <v>12414</v>
       </c>
       <c r="D33" t="n">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="E33" t="n">
-        <v>3148</v>
+        <v>3174</v>
       </c>
       <c r="F33" t="n">
         <v>131</v>
       </c>
       <c r="G33" t="n">
-        <v>25.61</v>
+        <v>25.57</v>
       </c>
       <c r="H33" t="n">
-        <v>25.59</v>
+        <v>25.49</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
@@ -2137,25 +2137,25 @@
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C35" t="n">
-        <v>74529</v>
+        <v>75875</v>
       </c>
       <c r="D35" t="n">
-        <v>1398</v>
+        <v>1420</v>
       </c>
       <c r="E35" t="n">
-        <v>11900</v>
+        <v>12230</v>
       </c>
       <c r="F35" t="n">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="G35" t="n">
-        <v>23.78</v>
+        <v>23.82</v>
       </c>
       <c r="H35" t="n">
-        <v>33.06</v>
+        <v>32.92</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
@@ -2164,10 +2164,10 @@
         <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>50048</v>
+        <v>51350</v>
       </c>
       <c r="L35" t="n">
-        <v>1349</v>
+        <v>1370</v>
       </c>
       <c r="M35" t="n">
         <v>2179622</v>
@@ -2188,25 +2188,25 @@
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C36" t="n">
-        <v>147865</v>
+        <v>148452</v>
       </c>
       <c r="D36" t="n">
-        <v>7026</v>
+        <v>7063</v>
       </c>
       <c r="E36" t="n">
-        <v>24783</v>
+        <v>24901</v>
       </c>
       <c r="F36" t="n">
-        <v>1958</v>
+        <v>1965</v>
       </c>
       <c r="G36" t="n">
-        <v>16.76</v>
+        <v>16.77</v>
       </c>
       <c r="H36" t="n">
-        <v>27.87</v>
+        <v>27.82</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
@@ -2235,16 +2235,16 @@
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C37" t="n">
-        <v>8052</v>
+        <v>8539</v>
       </c>
       <c r="D37" t="n">
         <v>94</v>
       </c>
       <c r="E37" t="n">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="F37" t="n">
         <v>1</v>
@@ -2282,25 +2282,25 @@
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C38" t="n">
-        <v>38569</v>
+        <v>39133</v>
       </c>
       <c r="D38" t="n">
-        <v>1474</v>
+        <v>1477</v>
       </c>
       <c r="E38" t="n">
-        <v>7928</v>
+        <v>8000</v>
       </c>
       <c r="F38" t="n">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G38" t="n">
-        <v>20.56</v>
+        <v>20.44</v>
       </c>
       <c r="H38" t="n">
-        <v>8.48</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="I38" t="b">
         <v>1</v>
@@ -2329,22 +2329,22 @@
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C39" t="n">
-        <v>110137</v>
+        <v>110338</v>
       </c>
       <c r="D39" t="n">
-        <v>8198</v>
+        <v>8213</v>
       </c>
       <c r="E39" t="n">
-        <v>10370</v>
+        <v>10400</v>
       </c>
       <c r="F39" t="n">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="G39" t="n">
-        <v>9.42</v>
+        <v>9.43</v>
       </c>
       <c r="H39" t="n">
         <v>8.18</v>
@@ -2376,25 +2376,25 @@
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C40" t="n">
-        <v>12436</v>
+        <v>12577</v>
       </c>
       <c r="D40" t="n">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E40" t="n">
-        <v>3592</v>
+        <v>3635</v>
       </c>
       <c r="F40" t="n">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G40" t="n">
-        <v>31.12</v>
+        <v>31.14</v>
       </c>
       <c r="H40" t="n">
-        <v>40.17</v>
+        <v>40.5</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
@@ -2403,10 +2403,10 @@
         <v>0</v>
       </c>
       <c r="K40" t="n">
-        <v>11541</v>
+        <v>11673</v>
       </c>
       <c r="L40" t="n">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="M40" t="n">
         <v>252321</v>
@@ -2427,13 +2427,13 @@
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>44009</v>
+        <v>44019</v>
       </c>
       <c r="C41" t="n">
-        <v>20261</v>
+        <v>24629</v>
       </c>
       <c r="D41" t="n">
-        <v>996</v>
+        <v>1042</v>
       </c>
       <c r="E41" t="n">
         <v>5758</v>
@@ -2481,13 +2481,13 @@
         <v>44019</v>
       </c>
       <c r="C42" t="n">
-        <v>31906</v>
+        <v>32042</v>
       </c>
       <c r="D42" t="n">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="E42" t="n">
-        <v>2868</v>
+        <v>2882</v>
       </c>
       <c r="F42" t="n">
         <v>36</v>
@@ -2496,7 +2496,7 @@
         <v>8.99</v>
       </c>
       <c r="H42" t="n">
-        <v>4.97</v>
+        <v>4.95</v>
       </c>
       <c r="I42" t="b">
         <v>1</v>

</xml_diff>